<commit_message>
update vervion of .net
</commit_message>
<xml_diff>
--- a/Excel Project/wwwroot/ExcelFiles/ClientData.xlsx
+++ b/Excel Project/wwwroot/ExcelFiles/ClientData.xlsx
@@ -56,6 +56,9 @@
   </x:si>
   <x:si>
     <x:t>tu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-03-30</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -486,6 +489,38 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
+    <x:row r="5" spans="1:10">
+      <x:c r="A5" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G5" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="J5" s="0">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>